<commit_message>
Column names changed to match the data
</commit_message>
<xml_diff>
--- a/Graphical Representation.xlsx
+++ b/Graphical Representation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,15 +74,6 @@
     <t>American</t>
   </si>
   <si>
-    <t>Negative Count</t>
-  </si>
-  <si>
-    <t>Nuetral Count</t>
-  </si>
-  <si>
-    <t>Positive Count</t>
-  </si>
-  <si>
     <t>Airline Name</t>
   </si>
   <si>
@@ -125,7 +116,16 @@
     <t>Reason</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>Statistics for different negative feedbacks</t>
+  </si>
+  <si>
+    <t>Negative feedback Count</t>
+  </si>
+  <si>
+    <t>Nuetral feedback Count</t>
+  </si>
+  <si>
+    <t>Positive feedback Count</t>
   </si>
 </sst>
 </file>
@@ -149,12 +149,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,9 +175,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,13 +313,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Negative Count</c:v>
+                  <c:v>Negative feedback Count</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nuetral Count</c:v>
+                  <c:v>Nuetral feedback Count</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Positive Count</c:v>
+                  <c:v>Positive feedback Count</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -587,7 +599,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Count</c:v>
+                  <c:v>Statistics for different negative feedbacks</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -942,7 +954,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Negative Count</c:v>
+                  <c:v>Negative feedback Count</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1032,7 +1044,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Nuetral Count</c:v>
+                  <c:v>Nuetral feedback Count</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1122,7 +1134,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Positive Count</c:v>
+                  <c:v>Positive feedback Count</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3436,7 +3448,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3447,18 +3459,18 @@
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3477,7 +3489,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3490,29 +3502,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>300</v>
@@ -3520,7 +3532,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>584</v>
@@ -3528,7 +3540,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>391</v>
@@ -3536,7 +3548,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>1447</v>
@@ -3544,7 +3556,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>31</v>
@@ -3552,7 +3564,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>237</v>
@@ -3560,7 +3572,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>235</v>
@@ -3568,7 +3580,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>798</v>
@@ -3576,7 +3588,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>348</v>
@@ -3584,7 +3596,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>72</v>
@@ -3592,7 +3604,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3609,8 +3621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3621,18 +3633,18 @@
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added description for the results.
</commit_message>
<xml_diff>
--- a/Graphical Representation.xlsx
+++ b/Graphical Representation.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Virgin America</t>
   </si>
@@ -113,9 +113,6 @@
     <t>longlines</t>
   </si>
   <si>
-    <t>Reason</t>
-  </si>
-  <si>
     <t>Statistics for different negative feedbacks</t>
   </si>
   <si>
@@ -127,12 +124,45 @@
   <si>
     <t>Positive feedback Count</t>
   </si>
+  <si>
+    <t>Mapreduce Problem:</t>
+  </si>
+  <si>
+    <t>Which airline has most negative feedback and which airline has most positive feedback</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Based on the data united airlines has most negative feedback and Southwest airline has most positive feedback</t>
+  </si>
+  <si>
+    <t>MapReduce Problem:</t>
+  </si>
+  <si>
+    <t>Reasons</t>
+  </si>
+  <si>
+    <t>Result:</t>
+  </si>
+  <si>
+    <t>Customer service is the main issue for the neagtive feedback based on the resultant data</t>
+  </si>
+  <si>
+    <t>which type of issues made customers to give most negative feedback and its values</t>
+  </si>
+  <si>
+    <t>What is the positive feedback values for the United Airlines</t>
+  </si>
+  <si>
+    <t>Based on the above values we can say total 1218 is the count for negative and 238 is the positive feedback count</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +177,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -175,14 +211,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3445,32 +3494,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3488,11 +3537,39 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="8"/>
       <c r="D9" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A9:B9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3500,10 +3577,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3515,11 +3592,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3608,6 +3685,26 @@
       </c>
       <c r="B12">
         <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3619,36 +3716,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -3662,7 +3759,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -3676,7 +3773,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -3690,7 +3787,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -3704,7 +3801,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -3718,7 +3815,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
@@ -3732,7 +3829,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8">
@@ -3746,7 +3843,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9">
@@ -3759,7 +3856,37 @@
         <v>139</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A15:B15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added changes in mapper3.py to remove header line
</commit_message>
<xml_diff>
--- a/Graphical Representation.xlsx
+++ b/Graphical Representation.xlsx
@@ -221,17 +221,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -295,7 +295,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -402,11 +401,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="150986632"/>
-        <c:axId val="150987024"/>
+        <c:axId val="167650952"/>
+        <c:axId val="167651344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150986632"/>
+        <c:axId val="167650952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150987024"/>
+        <c:crossAx val="167651344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150987024"/>
+        <c:axId val="167651344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,7 +507,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150986632"/>
+        <c:crossAx val="167650952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -602,7 +601,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -757,11 +755,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="150988200"/>
-        <c:axId val="150988592"/>
+        <c:axId val="167652520"/>
+        <c:axId val="167652912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150988200"/>
+        <c:axId val="167652520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,7 +802,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150988592"/>
+        <c:crossAx val="167652912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -812,7 +810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150988592"/>
+        <c:axId val="167652912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,7 +861,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150988200"/>
+        <c:crossAx val="167652520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1274,11 +1272,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="152161224"/>
-        <c:axId val="152161616"/>
+        <c:axId val="168326920"/>
+        <c:axId val="168327312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152161224"/>
+        <c:axId val="168326920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1319,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152161616"/>
+        <c:crossAx val="168327312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1329,26 +1327,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152161616"/>
+        <c:axId val="168327312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1380,7 +1364,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152161224"/>
+        <c:crossAx val="168326920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3537,10 +3521,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="7"/>
       <c r="D9" t="s">
         <v>7</v>
       </c>
@@ -3552,10 +3536,10 @@
       <c r="B10" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -3693,7 +3677,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3703,7 +3687,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3719,7 +3703,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+      <selection activeCell="A2" sqref="A2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3857,10 +3841,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -3869,16 +3853,16 @@
       <c r="B13" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Updated titles and graphs in Graphical Representation.xlsx
</commit_message>
<xml_diff>
--- a/Graphical Representation.xlsx
+++ b/Graphical Representation.xlsx
@@ -15,6 +15,7 @@
     <definedName name="_r1output" localSheetId="0">Sheet1!$A$1:$D$9</definedName>
     <definedName name="_r1output" localSheetId="2">Sheet3!$A$1:$D$9</definedName>
     <definedName name="_r2output_1" localSheetId="1">Sheet2!$A$2:$B$12</definedName>
+    <definedName name="_r3output" localSheetId="2">Sheet3!$A$2:$D$7</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -50,11 +51,21 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="4" name="r3output" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\s525743\Desktop\Tweet-Analysis---Airline-Sentiment\r3output.txt">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Virgin America</t>
   </si>
@@ -401,11 +412,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="167650952"/>
-        <c:axId val="167651344"/>
+        <c:axId val="134337648"/>
+        <c:axId val="134338032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="167650952"/>
+        <c:axId val="134337648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -448,7 +459,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167651344"/>
+        <c:crossAx val="134338032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -456,7 +467,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167651344"/>
+        <c:axId val="134338032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,7 +518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167650952"/>
+        <c:crossAx val="134337648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -755,11 +766,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="167652520"/>
-        <c:axId val="167652912"/>
+        <c:axId val="134027456"/>
+        <c:axId val="134027840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="167652520"/>
+        <c:axId val="134027456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,7 +813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167652912"/>
+        <c:crossAx val="134027840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -810,7 +821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167652912"/>
+        <c:axId val="134027840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,7 +872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167652520"/>
+        <c:crossAx val="134027456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -945,11 +956,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Ranges</a:t>
+              <a:t>Comparison of feedback for different</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of different types of feedback for airlines </a:t>
+              <a:t> airlines</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1018,65 +1029,53 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$A$2:$A$9</c:f>
+              <c:f>Sheet3!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Virgin America</c:v>
+                  <c:v>American</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>United</c:v>
+                  <c:v>Delta</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Southwest</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Delta</c:v>
+                  <c:v>US Airways</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>US Airways</c:v>
+                  <c:v>United</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>American</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Delta</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>American</c:v>
+                  <c:v>Virgin America</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$2:$B$9</c:f>
+              <c:f>Sheet3!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>85</c:v>
+                  <c:v>924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1218</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>573</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>483</c:v>
+                  <c:v>1159</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1159</c:v>
+                  <c:v>1218</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>886</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1108,65 +1107,53 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$A$2:$A$9</c:f>
+              <c:f>Sheet3!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Virgin America</c:v>
+                  <c:v>American</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>United</c:v>
+                  <c:v>Delta</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Southwest</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Delta</c:v>
+                  <c:v>US Airways</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>US Airways</c:v>
+                  <c:v>United</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>American</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Delta</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>American</c:v>
+                  <c:v>Virgin America</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$C$2:$C$9</c:f>
+              <c:f>Sheet3!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>90</c:v>
+                  <c:v>232</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>366</c:v>
+                  <c:v>451</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>451</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>201</c:v>
+                  <c:v>366</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>216</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1198,65 +1185,53 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$A$2:$A$9</c:f>
+              <c:f>Sheet3!$A$2:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Virgin America</c:v>
+                  <c:v>American</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>United</c:v>
+                  <c:v>Delta</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Southwest</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Delta</c:v>
+                  <c:v>US Airways</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>US Airways</c:v>
+                  <c:v>United</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>American</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Delta</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>American</c:v>
+                  <c:v>Virgin America</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$D$2:$D$9</c:f>
+              <c:f>Sheet3!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>238</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>288</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>123</c:v>
+                  <c:v>238</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>139</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1272,11 +1247,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="168326920"/>
-        <c:axId val="168327312"/>
+        <c:axId val="225741792"/>
+        <c:axId val="225741400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168326920"/>
+        <c:axId val="225741792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,7 +1294,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="168327312"/>
+        <c:crossAx val="225741400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1327,12 +1302,26 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168327312"/>
+        <c:axId val="225741400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1364,7 +1353,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="168326920"/>
+        <c:crossAx val="225741792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3148,20 +3137,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3188,6 +3177,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="r3output" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="r1output" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -3703,7 +3696,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D9"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3712,6 +3705,9 @@
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="9" max="10" width="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3729,35 +3725,35 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>85</v>
+        <v>924</v>
       </c>
       <c r="C2">
-        <v>90</v>
+        <v>232</v>
       </c>
       <c r="D2">
-        <v>64</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>1218</v>
+        <v>484</v>
       </c>
       <c r="C3">
-        <v>366</v>
+        <v>451</v>
       </c>
       <c r="D3">
-        <v>238</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -3771,73 +3767,45 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>483</v>
+        <v>1159</v>
       </c>
       <c r="C5">
-        <v>451</v>
+        <v>201</v>
       </c>
       <c r="D5">
-        <v>288</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
+      <c r="A6" t="s">
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>1159</v>
+        <v>1218</v>
       </c>
       <c r="C6">
-        <v>201</v>
+        <v>366</v>
       </c>
       <c r="D6">
-        <v>123</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
+      <c r="A7" t="s">
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="D7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>886</v>
-      </c>
-      <c r="C9">
-        <v>216</v>
-      </c>
-      <c r="D9">
-        <v>139</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>